<commit_message>
fix SMARTS file extension; minor bug fixes for other processes; add original version of ckan python chunked upload process
</commit_message>
<xml_diff>
--- a/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/CEDEN_Benthic_Data_Dictionary.xlsx
+++ b/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/CEDEN_Benthic_Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\David\Open_Data_Project\__CA_DataPortal\CEDEN\data_dictionary_conversion\benthic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04068105-9DFE-4849-A492-BD6C49531AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{04068105-9DFE-4849-A492-BD6C49531AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C44973-128F-4B51-875C-F149FFAC713B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEDEN_Benthic_Data_Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="172">
   <si>
     <t>column</t>
   </si>
@@ -1038,6 +1038,9 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>BenthicLabEffort_AgencyCode</t>
   </si>
 </sst>
 </file>
@@ -1872,9 +1875,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1912,7 +1915,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2018,7 +2021,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2160,7 +2163,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2168,21 +2171,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2202,7 +2207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>110</v>
       </c>
@@ -2225,7 +2230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>
@@ -2248,7 +2253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
@@ -2271,7 +2276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -2294,7 +2299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
@@ -2363,7 +2368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -2386,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>61</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>129</v>
       </c>
@@ -2434,7 +2439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2480,7 +2485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -2503,7 +2508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2526,7 +2531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2549,7 +2554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2572,7 +2577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>99</v>
       </c>
@@ -2595,7 +2600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
@@ -2618,7 +2623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
@@ -2641,7 +2646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>118</v>
       </c>
@@ -2664,7 +2669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>106</v>
       </c>
@@ -2687,7 +2692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -2710,7 +2715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>69</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>80</v>
       </c>
@@ -2756,7 +2761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
@@ -2779,7 +2784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>92</v>
       </c>
@@ -2802,7 +2807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>108</v>
       </c>
@@ -2825,7 +2830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>78</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
@@ -2871,7 +2876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>90</v>
       </c>
@@ -2894,7 +2899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>94</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>123</v>
       </c>
@@ -2940,7 +2945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>101</v>
       </c>
@@ -2963,7 +2968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>85</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>83</v>
       </c>
@@ -3009,7 +3014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
@@ -3032,7 +3037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>125</v>
       </c>
@@ -3078,7 +3083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>81</v>
       </c>
@@ -3124,7 +3129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>119</v>
       </c>
@@ -3147,7 +3152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>121</v>
       </c>
@@ -3170,7 +3175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>21</v>
       </c>
@@ -3193,7 +3198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>24</v>
       </c>
@@ -3216,7 +3221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>127</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>115</v>
       </c>
@@ -3285,7 +3290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
@@ -3308,7 +3313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>75</v>
       </c>
@@ -3331,7 +3336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
@@ -3354,7 +3359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>130</v>
       </c>
@@ -3377,7 +3382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>131</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>132</v>
       </c>
@@ -3423,7 +3428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>133</v>
       </c>
@@ -3446,7 +3451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>134</v>
       </c>
@@ -3469,7 +3474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>135</v>
       </c>
@@ -3492,7 +3497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>136</v>
       </c>
@@ -3515,7 +3520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>137</v>
       </c>
@@ -3538,7 +3543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>138</v>
       </c>
@@ -3561,7 +3566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>139</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>140</v>
       </c>
@@ -3607,7 +3612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>35</v>
       </c>
@@ -3630,19 +3635,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="144.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>57</v>
+        <v>171</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="4" t="str" cm="1">
         <f t="array" ref="C64">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E64),"-")</f>
-        <v>Data Quality</v>
+        <v>-</v>
       </c>
       <c r="D64" s="5" t="str" cm="1">
         <f t="array" ref="D64">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E64),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="E64" s="2" t="e">
+        <f>MATCH(A64,Data_Dictionary_FromPDF!A:A,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="144.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="4" t="str" cm="1">
+        <f t="array" ref="C65">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E65),"-")</f>
+        <v>Data Quality</v>
+      </c>
+      <c r="D65" s="5" t="str" cm="1">
+        <f t="array" ref="D65">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E65),"-")</f>
         <v>Describes the overall quality of the record by taking the QACode, ResultQACode, ComplicanceCode, BatchVerificationCode, and special circumstances into account to assign it to one of the following categories:
 - "Metadata, QC record”- Not a measurement of environmental conditions
 - "Passed QC"- Data passed all QC checks     
@@ -3653,48 +3681,40 @@
 - "Reject Data"- Data was rejected by the project or data did not pass all critical QC checks. Data deemed unusable
 The assignments and categories are provisional. A working explanation of the data quality ranking can be found at the following link. This link is open to public comments as well: https://docs.google.com/spreadsheets/d/1q-tGulvO9jyT2dR9GGROdy89z3W6xulYaci5-ezWAe0/edit?usp=sharing</v>
       </c>
-      <c r="E64" s="2">
-        <f>MATCH(A64,Data_Dictionary_FromPDF!A:A,0)</f>
+      <c r="E65" s="2">
+        <f>MATCH(A65,Data_Dictionary_FromPDF!A:A,0)</f>
         <v>14</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="F65" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="4" t="str" cm="1">
-        <f t="array" ref="C65">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E65),"-")</f>
+      <c r="B66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="4" t="str" cm="1">
+        <f t="array" ref="C66">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E66),"-")</f>
         <v>Data Quality Indicator</v>
       </c>
-      <c r="D65" s="5" t="str" cm="1">
-        <f t="array" ref="D65">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E65),"-")</f>
+      <c r="D66" s="5" t="str" cm="1">
+        <f t="array" ref="D66">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E66),"-")</f>
         <v>Explains the reason for the DataQuality value by indicating which quality assurance check the data did not pass (e.g.
 BatchVerificationCode, ResultQACode, etc.). If this field contains “Special Rule,” this indicates that the data falls into a special circumstance that decreases data quality. This field is left blank for values "Metadata, QC record" and "Passed QC."
 The assignments and categories are provisional. A working explanation of the data quality ranking can be found at the following link. This link is open to public comments as well: https://docs.google.com/spreadsheets/d/1q-tGulvO9jyT2dR9GGROdy89z3W6xulYaci5-ezWAe0/edit?usp=sharing</v>
       </c>
-      <c r="E65" s="2">
-        <f>MATCH(A65,Data_Dictionary_FromPDF!A:A,0)</f>
+      <c r="E66" s="2">
+        <f>MATCH(A66,Data_Dictionary_FromPDF!A:A,0)</f>
         <v>15</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3702,7 +3722,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3710,7 +3730,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3718,7 +3738,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3726,7 +3746,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3734,7 +3754,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3742,7 +3762,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3750,9 +3770,17 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B65" xr:uid="{D8F1714E-C0DF-435C-A2D2-777A56403E05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B66" xr:uid="{D8F1714E-C0DF-435C-A2D2-777A56403E05}">
       <formula1>"text, numeric, timestamp"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3767,17 +3795,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="22.88671875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="95.109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>62</v>
       </c>
@@ -3792,7 +3820,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>69</v>
       </c>
@@ -3810,7 +3838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>72</v>
       </c>
@@ -3828,7 +3856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
@@ -3846,7 +3874,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>78</v>
       </c>
@@ -3864,7 +3892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
@@ -3882,7 +3910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>80</v>
       </c>
@@ -3900,7 +3928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>44</v>
       </c>
@@ -3918,7 +3946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>27</v>
       </c>
@@ -3936,7 +3964,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -3954,7 +3982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -3972,7 +4000,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
@@ -3990,7 +4018,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
@@ -4008,7 +4036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="168" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>57</v>
       </c>
@@ -4023,10 +4051,10 @@
       </c>
       <c r="E14" s="6">
         <f>MATCH(A14,CEDEN_Benthic_Data_Dictionary!A:A,0)</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>59</v>
       </c>
@@ -4041,10 +4069,10 @@
       </c>
       <c r="E15" s="6">
         <f>MATCH(A15,CEDEN_Benthic_Data_Dictionary!A:A,0)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>61</v>
       </c>
@@ -4062,7 +4090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>85</v>
       </c>
@@ -4080,7 +4108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>88</v>
       </c>
@@ -4098,7 +4126,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>90</v>
       </c>
@@ -4116,7 +4144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>92</v>
       </c>
@@ -4134,7 +4162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>94</v>
       </c>
@@ -4152,7 +4180,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>96</v>
       </c>
@@ -4170,7 +4198,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>99</v>
       </c>
@@ -4188,7 +4216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>52</v>
       </c>
@@ -4206,7 +4234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>30</v>
       </c>
@@ -4224,7 +4252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>46</v>
       </c>
@@ -4242,7 +4270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>101</v>
       </c>
@@ -4260,7 +4288,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>19</v>
       </c>
@@ -4278,7 +4306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
         <v>48</v>
       </c>
@@ -4296,7 +4324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>103</v>
       </c>
@@ -4314,7 +4342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
         <v>105</v>
       </c>
@@ -4332,7 +4360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>106</v>
       </c>
@@ -4350,7 +4378,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>108</v>
       </c>
@@ -4368,7 +4396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>110</v>
       </c>
@@ -4386,7 +4414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
         <v>112</v>
       </c>
@@ -4404,7 +4432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>113</v>
       </c>
@@ -4422,7 +4450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
         <v>41</v>
       </c>
@@ -4440,7 +4468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>115</v>
       </c>
@@ -4458,7 +4486,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
         <v>116</v>
       </c>
@@ -4476,7 +4504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>38</v>
       </c>
@@ -4494,7 +4522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
         <v>14</v>
       </c>
@@ -4512,7 +4540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>54</v>
       </c>
@@ -4530,7 +4558,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A43" s="29" t="s">
         <v>118</v>
       </c>
@@ -4548,7 +4576,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>119</v>
       </c>
@@ -4566,7 +4594,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
         <v>121</v>
       </c>
@@ -4584,7 +4612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>123</v>
       </c>
@@ -4602,7 +4630,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" s="29" t="s">
         <v>12</v>
       </c>
@@ -4620,7 +4648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>10</v>
       </c>
@@ -4638,7 +4666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
         <v>125</v>
       </c>
@@ -4656,7 +4684,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>33</v>
       </c>
@@ -4674,7 +4702,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A51" s="29" t="s">
         <v>24</v>
       </c>
@@ -4692,7 +4720,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>127</v>
       </c>
@@ -4710,7 +4738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="45"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
@@ -4762,9 +4790,9 @@
       <selection activeCell="B65" sqref="B2:B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4778,7 +4806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -4786,7 +4814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -4794,7 +4822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4802,7 +4830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4810,7 +4838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4818,7 +4846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4826,7 +4854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -4834,7 +4862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4842,7 +4870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -4850,7 +4878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -4858,7 +4886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4866,7 +4894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4874,7 +4902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -4882,7 +4910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -4890,7 +4918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4898,7 +4926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -4906,7 +4934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -4914,7 +4942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4922,7 +4950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -4930,7 +4958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -4938,7 +4966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -4946,7 +4974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -4954,7 +4982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -4962,7 +4990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -4970,7 +4998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4978,7 +5006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -4986,7 +5014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -4994,7 +5022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -5002,7 +5030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -5010,7 +5038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -5018,7 +5046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -5026,7 +5054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -5034,7 +5062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -5042,7 +5070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -5050,7 +5078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -5058,7 +5086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -5066,7 +5094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -5074,7 +5102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -5082,7 +5110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -5090,7 +5118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -5098,7 +5126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -5106,7 +5134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -5114,7 +5142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -5122,7 +5150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -5130,7 +5158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -5138,7 +5166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -5146,7 +5174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -5154,7 +5182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -5162,7 +5190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -5170,7 +5198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -5178,7 +5206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -5186,7 +5214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -5194,7 +5222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -5202,7 +5230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -5210,7 +5238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5218,7 +5246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -5226,7 +5254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -5234,7 +5262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -5242,7 +5270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>138</v>
       </c>
@@ -5250,7 +5278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -5258,7 +5286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -5266,7 +5294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -5274,7 +5302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -5282,7 +5310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
minor updates, primarily revising data dictionary tools and adding new resources
</commit_message>
<xml_diff>
--- a/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/CEDEN_Benthic_Data_Dictionary.xlsx
+++ b/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/CEDEN_Benthic_Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/CEDEN/data_dictionaries/data_dictionary_conversion/benthic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{04068105-9DFE-4849-A492-BD6C49531AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFB1E00-F0F8-4F00-93E6-3DE537F0F5B0}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{04068105-9DFE-4849-A492-BD6C49531AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0F36D68-5810-42D1-A4D4-4A0AEFFF3151}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEDEN_Benthic_Data_Dictionary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="177">
   <si>
     <t>column</t>
   </si>
@@ -1038,6 +1038,21 @@
       </rPr>
       <t>http://ceden.org/CEDEN_Checker/Checker/DisplayCEDENLookUp.php?List=VariableCodesLookUp</t>
     </r>
+  </si>
+  <si>
+    <t>ProgramCode</t>
+  </si>
+  <si>
+    <t>ParentProjectCode</t>
+  </si>
+  <si>
+    <t>Unique code applied to the result which describes any special conditions, situations or outliers occurring during or prior to lab sorting. Default value equals NR if unknown.</t>
+  </si>
+  <si>
+    <t>Comments related to lab sorting or sample processing.</t>
+  </si>
+  <si>
+    <t>Refers to the percent of the sample that was counted.</t>
   </si>
 </sst>
 </file>
@@ -2172,23 +2187,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:D56"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>110</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>
@@ -2254,7 +2269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
@@ -2277,7 +2292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -2300,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2323,7 +2338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2346,7 +2361,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -2392,7 +2407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>61</v>
       </c>
@@ -2415,7 +2430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>129</v>
       </c>
@@ -2438,7 +2453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2461,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2484,7 +2499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -2507,7 +2522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2530,7 +2545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2553,7 +2568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2576,7 +2591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>99</v>
       </c>
@@ -2599,7 +2614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
@@ -2622,7 +2637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
@@ -2645,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>118</v>
       </c>
@@ -2668,7 +2683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>106</v>
       </c>
@@ -2691,7 +2706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -2714,7 +2729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>69</v>
       </c>
@@ -2737,7 +2752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>80</v>
       </c>
@@ -2760,7 +2775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
@@ -2783,7 +2798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>92</v>
       </c>
@@ -2806,7 +2821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>108</v>
       </c>
@@ -2829,7 +2844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>78</v>
       </c>
@@ -2852,7 +2867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
@@ -2875,7 +2890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>90</v>
       </c>
@@ -2898,7 +2913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>94</v>
       </c>
@@ -2921,7 +2936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>123</v>
       </c>
@@ -2944,7 +2959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>101</v>
       </c>
@@ -2967,7 +2982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>85</v>
       </c>
@@ -2990,7 +3005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>83</v>
       </c>
@@ -3013,7 +3028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
@@ -3036,7 +3051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
@@ -3059,7 +3074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>125</v>
       </c>
@@ -3082,7 +3097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
@@ -3105,7 +3120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>81</v>
       </c>
@@ -3128,7 +3143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>119</v>
       </c>
@@ -3151,7 +3166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>121</v>
       </c>
@@ -3174,7 +3189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>21</v>
       </c>
@@ -3197,7 +3212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -3243,7 +3258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>127</v>
       </c>
@@ -3266,7 +3281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>115</v>
       </c>
@@ -3289,7 +3304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
@@ -3312,7 +3327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>75</v>
       </c>
@@ -3335,7 +3350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
@@ -3358,7 +3373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>130</v>
       </c>
@@ -3380,8 +3395,11 @@
       <c r="F52" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>131</v>
       </c>
@@ -3403,8 +3421,11 @@
       <c r="F53" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>132</v>
       </c>
@@ -3426,8 +3447,11 @@
       <c r="F54" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>133</v>
       </c>
@@ -3450,7 +3474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>134</v>
       </c>
@@ -3473,7 +3497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>135</v>
       </c>
@@ -3496,7 +3520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>136</v>
       </c>
@@ -3519,7 +3543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>137</v>
       </c>
@@ -3542,7 +3566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>138</v>
       </c>
@@ -3565,7 +3589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>139</v>
       </c>
@@ -3588,7 +3612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>140</v>
       </c>
@@ -3611,7 +3635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>35</v>
       </c>
@@ -3634,7 +3658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>168</v>
       </c>
@@ -3657,19 +3681,65 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="4" t="str" cm="1">
         <f t="array" ref="C65">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E65),"-")</f>
-        <v>Data Quality</v>
+        <v>-</v>
       </c>
       <c r="D65" s="5" t="str" cm="1">
         <f t="array" ref="D65">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E65),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="E65" s="2" t="e">
+        <f>MATCH(A65,Data_Dictionary_FromPDF!A:A,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="4" t="str" cm="1">
+        <f t="array" ref="C66">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E66),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D66" s="5" t="str" cm="1">
+        <f t="array" ref="D66">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E66),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="E66" s="2" t="e">
+        <f>MATCH(A66,Data_Dictionary_FromPDF!A:A,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="168.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="4" t="str" cm="1">
+        <f t="array" ref="C67">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E67),"-")</f>
+        <v>Data Quality</v>
+      </c>
+      <c r="D67" s="5" t="str" cm="1">
+        <f t="array" ref="D67">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E67),"-")</f>
         <v>Describes the overall quality of the record by taking the QACode, ResultQACode, ComplicanceCode, BatchVerificationCode, and special circumstances into account to assign it to one of the following categories:
 - "Metadata, QC record”- Not a measurement of environmental conditions
 - "Passed QC"- Data passed all QC checks     
@@ -3680,55 +3750,39 @@
 - "Reject Data"- Data was rejected by the project or data did not pass all critical QC checks. Data deemed unusable
 The assignments and categories are provisional. A working explanation of the data quality ranking can be found at the following link. This link is open to public comments as well: https://docs.google.com/spreadsheets/d/1q-tGulvO9jyT2dR9GGROdy89z3W6xulYaci5-ezWAe0/edit?usp=sharing</v>
       </c>
-      <c r="E65" s="2">
-        <f>MATCH(A65,Data_Dictionary_FromPDF!A:A,0)</f>
+      <c r="E67" s="2">
+        <f>MATCH(A67,Data_Dictionary_FromPDF!A:A,0)</f>
         <v>14</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="F67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="84.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="4" t="str" cm="1">
-        <f t="array" ref="C66">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E66),"-")</f>
+      <c r="B68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="4" t="str" cm="1">
+        <f t="array" ref="C68">IFERROR(INDEX(Data_Dictionary_FromPDF!B:B,E68),"-")</f>
         <v>Data Quality Indicator</v>
       </c>
-      <c r="D66" s="5" t="str" cm="1">
-        <f t="array" ref="D66">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E66),"-")</f>
+      <c r="D68" s="5" t="str" cm="1">
+        <f t="array" ref="D68">IFERROR(INDEX(Data_Dictionary_FromPDF!D:D,E68),"-")</f>
         <v>Explains the reason for the DataQuality value by indicating which quality assurance check the data did not pass (e.g. BatchVerificationCode, ResultQACode, etc.). If this field contains “Special Rule,” this indicates that the data falls into a special circumstance that decreases data quality. This field is left blank for values "Metadata, QC record" and "Passed QC."
 The assignments and categories are provisional. A working explanation of the data quality ranking can be found at the following link. This link is open to public comments as well: https://docs.google.com/spreadsheets/d/1q-tGulvO9jyT2dR9GGROdy89z3W6xulYaci5-ezWAe0/edit?usp=sharing</v>
       </c>
-      <c r="E66" s="2">
-        <f>MATCH(A66,Data_Dictionary_FromPDF!A:A,0)</f>
+      <c r="E68" s="2">
+        <f>MATCH(A68,Data_Dictionary_FromPDF!A:A,0)</f>
         <v>15</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3736,7 +3790,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3744,7 +3798,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3752,7 +3806,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3760,7 +3814,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3768,7 +3822,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -3776,9 +3830,25 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B66" xr:uid="{D8F1714E-C0DF-435C-A2D2-777A56403E05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B68" xr:uid="{D8F1714E-C0DF-435C-A2D2-777A56403E05}">
       <formula1>"text, numeric, timestamp"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3795,17 +3865,17 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="22.88671875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="95.109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>62</v>
       </c>
@@ -3820,7 +3890,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>69</v>
       </c>
@@ -3838,7 +3908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>72</v>
       </c>
@@ -3856,7 +3926,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
@@ -3874,7 +3944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>78</v>
       </c>
@@ -3892,7 +3962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
@@ -3910,7 +3980,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>80</v>
       </c>
@@ -3928,7 +3998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>44</v>
       </c>
@@ -3946,7 +4016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>27</v>
       </c>
@@ -3964,7 +4034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -3982,7 +4052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -4000,7 +4070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
@@ -4018,7 +4088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
@@ -4036,7 +4106,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="192" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="168" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>57</v>
       </c>
@@ -4051,10 +4121,10 @@
       </c>
       <c r="E14" s="6">
         <f>MATCH(A14,CEDEN_Benthic_Data_Dictionary!A:A,0)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="96" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="84" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>59</v>
       </c>
@@ -4069,10 +4139,10 @@
       </c>
       <c r="E15" s="6">
         <f>MATCH(A15,CEDEN_Benthic_Data_Dictionary!A:A,0)</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>61</v>
       </c>
@@ -4090,7 +4160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>85</v>
       </c>
@@ -4108,7 +4178,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>88</v>
       </c>
@@ -4126,7 +4196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>90</v>
       </c>
@@ -4144,7 +4214,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>92</v>
       </c>
@@ -4162,7 +4232,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>94</v>
       </c>
@@ -4180,7 +4250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>96</v>
       </c>
@@ -4198,7 +4268,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>99</v>
       </c>
@@ -4216,7 +4286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>52</v>
       </c>
@@ -4234,7 +4304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>30</v>
       </c>
@@ -4252,7 +4322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>46</v>
       </c>
@@ -4270,7 +4340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>101</v>
       </c>
@@ -4288,7 +4358,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>19</v>
       </c>
@@ -4306,7 +4376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
         <v>48</v>
       </c>
@@ -4324,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>103</v>
       </c>
@@ -4342,7 +4412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
         <v>105</v>
       </c>
@@ -4360,7 +4430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>106</v>
       </c>
@@ -4378,7 +4448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>108</v>
       </c>
@@ -4396,7 +4466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>110</v>
       </c>
@@ -4414,7 +4484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
         <v>112</v>
       </c>
@@ -4432,7 +4502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>113</v>
       </c>
@@ -4450,7 +4520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
         <v>41</v>
       </c>
@@ -4468,7 +4538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>115</v>
       </c>
@@ -4486,7 +4556,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
         <v>116</v>
       </c>
@@ -4504,7 +4574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>38</v>
       </c>
@@ -4522,7 +4592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
         <v>14</v>
       </c>
@@ -4540,7 +4610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>54</v>
       </c>
@@ -4558,7 +4628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A43" s="29" t="s">
         <v>118</v>
       </c>
@@ -4576,7 +4646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>119</v>
       </c>
@@ -4594,7 +4664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
         <v>121</v>
       </c>
@@ -4612,7 +4682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>123</v>
       </c>
@@ -4630,7 +4700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" s="29" t="s">
         <v>12</v>
       </c>
@@ -4648,7 +4718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>10</v>
       </c>
@@ -4666,7 +4736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
         <v>125</v>
       </c>
@@ -4684,7 +4754,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>33</v>
       </c>
@@ -4702,7 +4772,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A51" s="29" t="s">
         <v>24</v>
       </c>
@@ -4720,7 +4790,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>127</v>
       </c>
@@ -4738,7 +4808,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="45"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
@@ -4790,9 +4860,9 @@
       <selection activeCell="B65" sqref="B2:B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +4876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -4814,7 +4884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -4822,7 +4892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4830,7 +4900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4838,7 +4908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4846,7 +4916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4854,7 +4924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -4862,7 +4932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4870,7 +4940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -4878,7 +4948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -4886,7 +4956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4894,7 +4964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4902,7 +4972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -4910,7 +4980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -4918,7 +4988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4926,7 +4996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -4934,7 +5004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -4942,7 +5012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4950,7 +5020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -4958,7 +5028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -4966,7 +5036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -4974,7 +5044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -4982,7 +5052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -4990,7 +5060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -4998,7 +5068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -5006,7 +5076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -5014,7 +5084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -5022,7 +5092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -5030,7 +5100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -5038,7 +5108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -5046,7 +5116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -5054,7 +5124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -5062,7 +5132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -5070,7 +5140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -5078,7 +5148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -5086,7 +5156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -5094,7 +5164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -5102,7 +5172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -5110,7 +5180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -5118,7 +5188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -5126,7 +5196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -5134,7 +5204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -5142,7 +5212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -5150,7 +5220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -5158,7 +5228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -5166,7 +5236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -5174,7 +5244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -5182,7 +5252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -5190,7 +5260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -5198,7 +5268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -5206,7 +5276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -5214,7 +5284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -5222,7 +5292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -5230,7 +5300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -5238,7 +5308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5246,7 +5316,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -5254,7 +5324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -5262,7 +5332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -5270,7 +5340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>138</v>
       </c>
@@ -5278,7 +5348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -5286,7 +5356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -5294,7 +5364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -5302,7 +5372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -5310,7 +5380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>59</v>
       </c>

</xml_diff>